<commit_message>
Versión para Abril - Diciembre 2024
</commit_message>
<xml_diff>
--- a/AAA - Revision Asignacion con ajuste Manual.xlsx
+++ b/AAA - Revision Asignacion con ajuste Manual.xlsx
@@ -552,13 +552,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>6.224379325864566</v>
+        <v>6.224379325864565</v>
       </c>
       <c r="G2" t="n">
-        <v>8.928571428571429</v>
+        <v>20</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0.3415730337078651</v>
+        <v>0.2512396694214876</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -615,10 +615,10 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>6.224379325864566</v>
+        <v>6.224379325864565</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>6.280334269970441</v>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>6.280334269970441</v>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>6.344804096875039</v>
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>6.344804096875039</v>
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>6.344804096875039</v>
@@ -993,7 +993,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>6.613631110948924</v>
@@ -1056,13 +1056,13 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>6.706078409906459</v>
       </c>
       <c r="G10" t="n">
-        <v>10.71428571428572</v>
+        <v>30</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1089,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>0.2841121495327102</v>
+        <v>0.2512396694214876</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
@@ -1119,7 +1119,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
         <v>6.728277925774551</v>
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>6.928073568587381</v>
@@ -1245,13 +1245,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>7.131822549842476</v>
       </c>
       <c r="G13" t="n">
-        <v>80.35714285714286</v>
+        <v>50</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>0.3304347826086956</v>
+        <v>0.2512396694214876</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -1308,7 +1308,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>7.214842657129998</v>
@@ -1371,7 +1371,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>7.214842657129998</v>

</xml_diff>